<commit_message>
Addition of Data to Land Use Data
CSpULApYbP, CiLVpUAAbP, and FoFObE all now have data.
</commit_message>
<xml_diff>
--- a/InputData/land/FoFObE/Fraction of Forests Owned by Entity.xlsx
+++ b/InputData/land/FoFObE/Fraction of Forests Owned by Entity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anima\Desktop\Models\eps-brazil-cpl\InputData\land\FoFObE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4C1A6C-64A3-4BB5-8D88-3077FCCA9CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DA69B1-89D4-4F02-9F8A-89CA12AE9178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>FoFObE Fraction of Forests Owned by Entity</t>
   </si>
@@ -58,33 +58,9 @@
     <t>Ownership of Forest Land (million hectares)</t>
   </si>
   <si>
-    <t>U.S. Forest Service</t>
-  </si>
-  <si>
-    <t>U.S. Forest Facts and Historical Trends</t>
-  </si>
-  <si>
-    <t>http://www.fia.fs.fed.us/library/briefings-summaries-overviews/docs/ForestFactsMetric.pdf</t>
-  </si>
-  <si>
-    <t>Page 6</t>
-  </si>
-  <si>
     <t>government</t>
   </si>
   <si>
-    <t>The amount of government-owned forest is provided in the table.</t>
-  </si>
-  <si>
-    <t>We assume that all privately-owned forest used for timber land is owned</t>
-  </si>
-  <si>
-    <t>by industry, and half of the remaining privately-owned forest land is owned</t>
-  </si>
-  <si>
-    <t>by industry.  The remainder is owned by consumers.</t>
-  </si>
-  <si>
     <t>foreign entities</t>
   </si>
   <si>
@@ -97,12 +73,6 @@
     <t>domestic industries</t>
   </si>
   <si>
-    <t>Notes - US</t>
-  </si>
-  <si>
-    <t>Forest Area (1000 ha)</t>
-  </si>
-  <si>
     <t>Global Forest Resources Assessment 2020</t>
   </si>
   <si>
@@ -115,13 +85,106 @@
     <t>Notes - Brazil</t>
   </si>
   <si>
-    <t>Even though the report is from 2020, the land data it provides is from 2015</t>
-  </si>
-  <si>
     <t>private ownership</t>
   </si>
   <si>
     <t>Forest Resources Assessment</t>
+  </si>
+  <si>
+    <t>US News</t>
+  </si>
+  <si>
+    <t>Logging</t>
+  </si>
+  <si>
+    <t>Area (ha)</t>
+  </si>
+  <si>
+    <t>Mongabay</t>
+  </si>
+  <si>
+    <t>Ranching</t>
+  </si>
+  <si>
+    <t>Area (mi^2)</t>
+  </si>
+  <si>
+    <t>Mining</t>
+  </si>
+  <si>
+    <t>Area (km^2)</t>
+  </si>
+  <si>
+    <t>Legality Risk Dashboard</t>
+  </si>
+  <si>
+    <t>Illegal Logging</t>
+  </si>
+  <si>
+    <t>Unit Conversions</t>
+  </si>
+  <si>
+    <t>acre/km^2</t>
+  </si>
+  <si>
+    <t>Conversions via housing.com/calculators/</t>
+  </si>
+  <si>
+    <t>acre/ha</t>
+  </si>
+  <si>
+    <t>acre/mi^2</t>
+  </si>
+  <si>
+    <t>In acres</t>
+  </si>
+  <si>
+    <t>total area</t>
+  </si>
+  <si>
+    <t>Total Area</t>
+  </si>
+  <si>
+    <t>Total (2020)</t>
+  </si>
+  <si>
+    <t>Forest Area (ha)</t>
+  </si>
+  <si>
+    <t>https://www.theguardian.com/environment/2023/jun/02/mining-cattle-ranching-soya-farming-corporations-dominate-amazon</t>
+  </si>
+  <si>
+    <t>Like in the US report, foreign entities at 0. Most of the major sources of exploitation are Brazilian in origin (see link below)</t>
+  </si>
+  <si>
+    <t>Accordingly, logging and mining deemed domestic industry, ranching and illegal forestry deemed labour and consumers</t>
+  </si>
+  <si>
+    <t>"Brazil to Allow Miles of Selective Logging in Effort to Preserve the Amazon"</t>
+  </si>
+  <si>
+    <t>https://www.usnews.com/news/business/articles/2024-07-23/brazil-to-allow-miles-of-selective-logging-in-effort-to-preserve-the-amazon#:~:text=Currently%2C%20there%20are%2022%20such,Finance%20to%20address%20climate%20change.</t>
+  </si>
+  <si>
+    <t>US News, Associated Press</t>
+  </si>
+  <si>
+    <t>"Mining activity causing nearly 10 percent of Amazon deforestation"</t>
+  </si>
+  <si>
+    <t>Mongabay, Zoe Sullivan</t>
+  </si>
+  <si>
+    <t>https://news.mongabay.com/2017/11/mining-activity-causing-nearly-10-percent-of-amazon-deforestation/#:~:text=Also%2C%20just%20as%20clearly%2C%20mining,maimed%20by%20the%20freight%20trains.</t>
+  </si>
+  <si>
+    <t>"Beef consumption fuels rainforest destruction"</t>
+  </si>
+  <si>
+    <t>Mongabay, Rhett Butler</t>
+  </si>
+  <si>
+    <t>https://news.mongabay.com/2009/02/beef-consumption-fuels-rainforest-destruction/</t>
   </si>
 </sst>
 </file>
@@ -131,7 +194,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,14 +206,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -173,20 +228,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -194,10 +244,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -500,13 +552,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -517,91 +572,143 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B4" s="3">
-        <v>2001</v>
+      <c r="B4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>12</v>
+      <c r="B5">
+        <v>2015</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B6" s="4" t="s">
-        <v>13</v>
+      <c r="B6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B10">
-        <v>2015</v>
+      <c r="B10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>27</v>
+      <c r="B11">
+        <v>2024</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" s="8" t="s">
-        <v>30</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>247.10538149999999</v>
+      </c>
+      <c r="C33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B34">
+        <v>2.4710538149999999</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B35">
+        <v>640</v>
+      </c>
+      <c r="C35" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -609,7 +716,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -622,7 +731,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -762,45 +871,200 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDDAD4E1-7378-4FBE-BFA8-7480C06A880A}">
-  <dimension ref="A2:B5"/>
+  <dimension ref="A2:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>2015</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2">
+        <v>2024</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>2009</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2">
+        <v>2017</v>
+      </c>
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4">
-        <v>281102.40999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6">
+        <f>1000*281102.41</f>
+        <v>281102410</v>
+      </c>
+      <c r="N4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6">
+        <f>1000*222782.39</f>
+        <v>222782390</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5">
+        <v>1300000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5">
+        <v>214000</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5">
+        <f>1.65*0.6*10^6</f>
+        <v>989999.99999999988</v>
+      </c>
+      <c r="M5" t="s">
         <v>31</v>
       </c>
-      <c r="B5">
-        <v>222782.39</v>
+      <c r="N5">
+        <f>55*10^6</f>
+        <v>55000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>496619620</v>
+      </c>
+      <c r="M6" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6">
+        <f>496.6*10^6</f>
+        <v>496600000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="6">
+        <f>B4*About!B34</f>
+        <v>694619182.63619411</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9">
+        <f>E5*About!B34</f>
+        <v>3212369.9594999999</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9">
+        <f>H5*About!B35</f>
+        <v>136960000</v>
+      </c>
+      <c r="J9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="6">
+        <f>K5*About!B33</f>
+        <v>244634327.68499997</v>
+      </c>
+      <c r="M9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="6">
+        <f>About!B34*N5</f>
+        <v>135907959.82499999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="6">
+        <f>B5*About!B34</f>
+        <v>550507274.72431779</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <f>B10/B12</f>
+        <v>0.4486153644784534</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="6">
+        <f>N6*About!B34</f>
+        <v>1227125324.529</v>
       </c>
     </row>
   </sheetData>
@@ -816,7 +1080,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -826,40 +1090,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="B1" s="7" t="s">
-        <v>22</v>
+      <c r="B1" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="5">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3">
         <f>SUM(Data_US!B3,Data_US!B7)/SUM(Data_US!B3,Data_US!B7,Data_US!B11,Data_US!B15)</f>
         <v>0.42384105960264901</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="5">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3">
         <f>SUM(Data_US!B11,Data_US!B16,Data_US!B18/2)/SUM(Data_US!B3,Data_US!B7,Data_US!B11,Data_US!B15)</f>
         <v>0.52814569536423839</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="5">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3">
         <f>(Data_US!B18/2)/SUM(Data_US!B3,Data_US!B7,Data_US!B11,Data_US!B15)</f>
         <v>4.8013245033112585E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>0</v>

</xml_diff>

<commit_message>
FoFObE update to computations
No change to data presented, the blue tab is just now updated to contain the Brazil data and the US data is deleted.
</commit_message>
<xml_diff>
--- a/InputData/land/FoFObE/Fraction of Forests Owned by Entity.xlsx
+++ b/InputData/land/FoFObE/Fraction of Forests Owned by Entity.xlsx
@@ -8,22 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anima\Desktop\Models\eps-brazil-cpl\InputData\land\FoFObE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DA69B1-89D4-4F02-9F8A-89CA12AE9178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A2FA24-15AA-4E56-8DD6-64824B0F9F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Data_US" sheetId="2" r:id="rId2"/>
-    <sheet name="Data_Brazil" sheetId="4" r:id="rId3"/>
-    <sheet name="FoFObE" sheetId="3" r:id="rId4"/>
+    <sheet name="Data_Brazil" sheetId="4" r:id="rId2"/>
+    <sheet name="FoFObE" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>FoFObE Fraction of Forests Owned by Entity</t>
   </si>
@@ -31,33 +30,6 @@
     <t>Source:</t>
   </si>
   <si>
-    <t>National Forest</t>
-  </si>
-  <si>
-    <t>Other public</t>
-  </si>
-  <si>
-    <t>Forest industry</t>
-  </si>
-  <si>
-    <t>Other private</t>
-  </si>
-  <si>
-    <t>Timber land</t>
-  </si>
-  <si>
-    <t>Reserved forest</t>
-  </si>
-  <si>
-    <t>Other forest</t>
-  </si>
-  <si>
-    <t>U.S.</t>
-  </si>
-  <si>
-    <t>Ownership of Forest Land (million hectares)</t>
-  </si>
-  <si>
     <t>government</t>
   </si>
   <si>
@@ -185,6 +157,15 @@
   </si>
   <si>
     <t>https://news.mongabay.com/2009/02/beef-consumption-fuels-rainforest-destruction/</t>
+  </si>
+  <si>
+    <t>Domestic Industry Fraction</t>
+  </si>
+  <si>
+    <t>Government Fraction</t>
+  </si>
+  <si>
+    <t>Labour Fraction</t>
   </si>
 </sst>
 </file>
@@ -231,16 +212,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -554,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
@@ -575,7 +550,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -585,22 +560,22 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -610,17 +585,17 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -630,17 +605,17 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -650,7 +625,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -658,36 +633,36 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="7" t="s">
-        <v>32</v>
+      <c r="A33" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="B33">
         <v>247.10538149999999</v>
       </c>
       <c r="C33" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E33" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -695,7 +670,7 @@
         <v>2.4710538149999999</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -703,7 +678,7 @@
         <v>640</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -713,168 +688,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDDAD4E1-7378-4FBE-BFA8-7480C06A880A}">
+  <dimension ref="A2:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="17.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="1">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDDAD4E1-7378-4FBE-BFA8-7480C06A880A}">
-  <dimension ref="A2:N12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -893,31 +711,31 @@
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>2015</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <v>2024</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H2">
         <v>2009</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="K2">
         <v>2017</v>
       </c>
       <c r="M2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="N2">
         <v>1999</v>
@@ -925,59 +743,59 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
         <f>1000*281102.41</f>
         <v>281102410</v>
       </c>
       <c r="N4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="6">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4">
         <f>1000*222782.39</f>
         <v>222782390</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E5">
         <v>1300000</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H5">
         <v>214000</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="K5">
         <f>1.65*0.6*10^6</f>
         <v>989999.99999999988</v>
       </c>
       <c r="M5" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="N5">
         <f>55*10^6</f>
@@ -986,13 +804,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>496619620</v>
       </c>
       <c r="M6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="N6">
         <f>496.6*10^6</f>
@@ -1001,70 +819,93 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="6">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4">
         <f>B4*About!B34</f>
         <v>694619182.63619411</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E9">
         <f>E5*About!B34</f>
         <v>3212369.9594999999</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H9">
         <f>H5*About!B35</f>
         <v>136960000</v>
       </c>
       <c r="J9" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="6">
+        <v>19</v>
+      </c>
+      <c r="K9" s="4">
         <f>K5*About!B33</f>
         <v>244634327.68499997</v>
       </c>
       <c r="M9" t="s">
-        <v>31</v>
-      </c>
-      <c r="N9" s="6">
+        <v>22</v>
+      </c>
+      <c r="N9" s="4">
         <f>About!B34*N5</f>
         <v>135907959.82499999</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="6">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4">
         <f>B5*About!B34</f>
         <v>550507274.72431779</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C11">
-        <f>B10/B12</f>
-        <v>0.4486153644784534</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="6">
+        <v>29</v>
+      </c>
+      <c r="B12" s="4">
         <f>N6*About!B34</f>
         <v>1227125324.529</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14">
+        <f>(E9+K9)/B12</f>
+        <v>0.20197341925090612</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15">
+        <f>(H9+N9)/B12</f>
+        <v>0.22236356333835194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16">
+        <f>B9/B12</f>
+        <v>0.56605398711236399</v>
       </c>
     </row>
   </sheetData>
@@ -1072,15 +913,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1090,40 +931,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="B1" s="5" t="s">
-        <v>14</v>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="3">
-        <f>SUM(Data_US!B3,Data_US!B7)/SUM(Data_US!B3,Data_US!B7,Data_US!B11,Data_US!B15)</f>
-        <v>0.42384105960264901</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <f>Data_Brazil!B16</f>
+        <v>0.56605398711236399</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="3">
-        <f>SUM(Data_US!B11,Data_US!B16,Data_US!B18/2)/SUM(Data_US!B3,Data_US!B7,Data_US!B11,Data_US!B15)</f>
-        <v>0.52814569536423839</v>
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <f>Data_Brazil!B14</f>
+        <v>0.20197341925090612</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="3">
-        <f>(Data_US!B18/2)/SUM(Data_US!B3,Data_US!B7,Data_US!B11,Data_US!B15)</f>
-        <v>4.8013245033112585E-2</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <f>Data_Brazil!B15</f>
+        <v>0.22236356333835194</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0</v>

</xml_diff>

<commit_message>
Update FoFObE with percentage
</commit_message>
<xml_diff>
--- a/InputData/land/FoFObE/Fraction of Forests Owned by Entity.xlsx
+++ b/InputData/land/FoFObE/Fraction of Forests Owned by Entity.xlsx
@@ -1,23 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anima\Desktop\Models\eps-brazil-cpl\InputData\land\FoFObE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ssy02/Desktop/Postdoc Projects/eps-brazil-cpl/InputData/land/FoFObE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A2FA24-15AA-4E56-8DD6-64824B0F9F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36832FD7-04DB-1540-B33D-A24320F304F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="21380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data_Brazil" sheetId="4" r:id="rId2"/>
     <sheet name="FoFObE" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -533,125 +546,125 @@
       <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.90625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>2024</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>2017</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>2009</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>23</v>
       </c>
@@ -665,7 +678,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B34">
         <v>2.4710538149999999</v>
       </c>
@@ -673,7 +686,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B35">
         <v>640</v>
       </c>
@@ -692,24 +705,24 @@
   <dimension ref="A2:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -741,7 +754,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>32</v>
       </c>
@@ -755,7 +768,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -767,7 +780,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -802,7 +815,7 @@
         <v>55000000</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -817,12 +830,12 @@
         <v>496600000</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -859,7 +872,7 @@
         <v>135907959.82499999</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -868,11 +881,11 @@
         <v>550507274.72431779</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -881,31 +894,31 @@
         <v>1227125324.529</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>45</v>
       </c>
       <c r="B14">
-        <f>(E9+K9)/B12</f>
-        <v>0.20197341925090612</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+        <f>ROUNDUP((E9+K9)/B12,2)</f>
+        <v>0.21000000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>47</v>
       </c>
       <c r="B15">
-        <f>(H9+N9)/B12</f>
-        <v>0.22236356333835194</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+        <f>ROUND((H9+N9)/B12,2)</f>
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>46</v>
       </c>
       <c r="B16">
-        <f>B9/B12</f>
-        <v>0.56605398711236399</v>
+        <f>ROUND((B9/B12),2)</f>
+        <v>0.56999999999999995</v>
       </c>
     </row>
   </sheetData>
@@ -918,57 +931,60 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.81640625" customWidth="1"/>
-    <col min="2" max="2" width="23.7265625" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2">
         <f>Data_Brazil!B16</f>
-        <v>0.56605398711236399</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2">
         <f>Data_Brazil!B14</f>
-        <v>0.20197341925090612</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.21000000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2">
         <f>Data_Brazil!B15</f>
-        <v>0.22236356333835194</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>0</v>
       </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>